<commit_message>
added new use case
</commit_message>
<xml_diff>
--- a/Hacktoberfest_Input.xlsx
+++ b/Hacktoberfest_Input.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anshul.choudhary@ibm.com/PycharmProjects/Auto-Opsi/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anshul.choudhary@ibm.com/PycharmProjects/Manipulating_Excel_Sheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CD27632A-306B-1546-B29A-EC595C0777DE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F0E7793F-B977-0C44-8EFC-3D9AABF9483A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13580" yWindow="7960" windowWidth="26040" windowHeight="14940" xr2:uid="{240A953C-158B-9649-AC89-6A8615E9C240}"/>
+    <workbookView xWindow="27040" yWindow="-20940" windowWidth="26040" windowHeight="14940" xr2:uid="{240A953C-158B-9649-AC89-6A8615E9C240}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
   <si>
     <t>Source</t>
   </si>
@@ -68,7 +68,16 @@
     <t>156.78.90.3</t>
   </si>
   <si>
-    <t>56.78.3.4</t>
+    <t>9.208.46.246
+9.208.48.81
+9.208.48.48</t>
+  </si>
+  <si>
+    <t>9.214.16.167</t>
+  </si>
+  <si>
+    <t>9.208.46.246,9.208.48.81,
+9.208.48.48</t>
   </si>
 </sst>
 </file>
@@ -122,11 +131,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -441,10 +453,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B463CD9-5D49-5A46-B22F-46878949AC3C}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A4" sqref="A3:A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -489,17 +501,31 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="51" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>10</v>
       </c>
-      <c r="C6" t="s">
-        <v>11</v>
+      <c r="C6" s="4" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>4</v>
+      </c>
+      <c r="C7" s="4"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>